<commit_message>
working version of schecule checker & calendar output
</commit_message>
<xml_diff>
--- a/23FQ CLSS Scheduling 022723.xlsx
+++ b/23FQ CLSS Scheduling 022723.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\git\Teaching\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{EDCD5C3E-68AB-4CF0-B862-177B995E4DD5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{927565C8-27CE-471D-B7DC-D8821C1F31C2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2340" yWindow="2340" windowWidth="24540" windowHeight="12120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-105" yWindow="2340" windowWidth="23610" windowHeight="12120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="23FQ" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="152" uniqueCount="80">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="159" uniqueCount="86">
   <si>
     <t>Term Code</t>
   </si>
@@ -279,13 +279,31 @@
   </si>
   <si>
     <t>X: CEEGR 4870-01</t>
+  </si>
+  <si>
+    <t>BANN 371</t>
+  </si>
+  <si>
+    <t>BANN 619</t>
+  </si>
+  <si>
+    <t>LEML 122</t>
+  </si>
+  <si>
+    <t>Gnanapragrasam</t>
+  </si>
+  <si>
+    <t>Riazi</t>
+  </si>
+  <si>
+    <t>Gnanapragasam</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="18" x14ac:knownFonts="1">
+  <fonts count="19" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -416,6 +434,12 @@
     <font>
       <sz val="11"/>
       <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -762,7 +786,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -770,6 +794,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1128,7 +1153,7 @@
   <dimension ref="A1:O21"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="77" zoomScaleNormal="77" workbookViewId="0">
-      <selection activeCell="G19" sqref="G19"/>
+      <selection activeCell="H2" sqref="H2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1138,7 +1163,7 @@
     <col min="4" max="4" width="28.5703125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="14.85546875" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="38.140625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="11.42578125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="18.140625" customWidth="1"/>
     <col min="8" max="8" width="15.85546875" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="15.42578125" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="11.7109375" customWidth="1"/>
@@ -1214,7 +1239,9 @@
       <c r="F2" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="G2" s="2"/>
+      <c r="G2" s="2" t="s">
+        <v>85</v>
+      </c>
       <c r="H2" s="2"/>
       <c r="I2" s="2" t="s">
         <v>20</v>
@@ -1248,7 +1275,9 @@
         <v>23</v>
       </c>
       <c r="G3" s="2"/>
-      <c r="H3" s="2"/>
+      <c r="H3" s="3" t="s">
+        <v>80</v>
+      </c>
       <c r="I3" s="2" t="s">
         <v>20</v>
       </c>
@@ -1418,7 +1447,9 @@
       <c r="F8" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="G8" s="2"/>
+      <c r="G8" s="2" t="s">
+        <v>84</v>
+      </c>
       <c r="H8" s="2"/>
       <c r="I8" s="2" t="s">
         <v>20</v>
@@ -1486,8 +1517,12 @@
       <c r="F10" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="G10" s="2"/>
-      <c r="H10" s="2"/>
+      <c r="G10" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="H10" s="2" t="s">
+        <v>81</v>
+      </c>
       <c r="I10" s="2" t="s">
         <v>20</v>
       </c>
@@ -1873,8 +1908,12 @@
       <c r="F21" s="2" t="s">
         <v>62</v>
       </c>
-      <c r="G21" s="2"/>
-      <c r="H21" s="2"/>
+      <c r="G21" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="H21" s="2" t="s">
+        <v>82</v>
+      </c>
       <c r="I21" s="2" t="s">
         <v>20</v>
       </c>

</xml_diff>